<commit_message>
change amount of items on left
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:E4"/>
+  <dimension ref="A0:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,18 +367,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="0"/>
+    <row r="0">
+      <c r="A0" t="inlineStr">
+        <is>
+          <t>치킨</t>
+        </is>
+      </c>
+      <c r="B0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="C0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="E0" t="inlineStr"/>
+    </row>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>양념치킨</t>
+          <t>삼겹살</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="n">
         <v>9000</v>
@@ -395,17 +411,17 @@
         <v>2500</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>2500</v>
+        <v>22500</v>
       </c>
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>김밥</t>
+          <t>대패삼겹살</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -422,20 +438,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>배추김치</t>
+          <t>양념치킨</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" t="n">
-        <v>8000</v>
+        <v>63000</v>
       </c>
       <c r="E4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>치킨</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>16000</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add count from center
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:E13"/>
+  <dimension ref="A0:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -368,242 +368,38 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="0">
-      <c r="A0" s="0" t="inlineStr">
+      <c r="A0" t="inlineStr">
         <is>
           <t>치즈김밥</t>
         </is>
       </c>
-      <c r="B0" s="0" t="n">
+      <c r="B0" t="n">
         <v>2500</v>
       </c>
-      <c r="C0" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D0" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E0" s="0" t="inlineStr"/>
+      <c r="C0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D0" t="n">
+        <v>25000</v>
+      </c>
+      <c r="E0" t="inlineStr"/>
     </row>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>김밥</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E1" s="0" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>대패삼겹살</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E2" s="0" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>치즈김밥</t>
         </is>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B1" t="n">
         <v>2500</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C1" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>12500</v>
-      </c>
-      <c r="E3" s="0" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>김밥</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="E4" s="0" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>닭볶음탕</t>
-        </is>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>18000</v>
-      </c>
-      <c r="E5" s="0" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>녹말요지</t>
-        </is>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>2200</v>
-      </c>
-      <c r="E6" s="0" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>접시100</t>
-        </is>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E7" s="0" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="inlineStr">
-        <is>
-          <t>삼겹살</t>
-        </is>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E8" s="0" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="inlineStr">
-        <is>
-          <t>대패삼겹살</t>
-        </is>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E9" s="0" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="inlineStr">
-        <is>
-          <t>치즈김밥</t>
-        </is>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>12500</v>
-      </c>
-      <c r="E10" s="0" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="inlineStr">
-        <is>
-          <t>김밥</t>
-        </is>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="E11" s="0" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="inlineStr">
-        <is>
-          <t>닭볶음탕</t>
-        </is>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>18000</v>
-      </c>
-      <c r="E12" s="0" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="inlineStr">
-        <is>
-          <t>식탁보</t>
-        </is>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E13" s="0" t="inlineStr"/>
+      <c r="D1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add c_click with many issues
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -359,79 +359,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>새우튀김</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2600</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>2600</v>
-      </c>
-      <c r="E2" s="0" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>닭볶음탕</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,88 +370,155 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>닭볶음탕</t>
+          <t>양념치킨</t>
         </is>
       </c>
       <c r="B1" s="0" t="n">
         <v>9000</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>9000</v>
+        <v>36000</v>
       </c>
       <c r="E1" s="0" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>새우튀김</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2600</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>닭볶음탕</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>2600</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E2" s="0" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A0:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="0">
+      <c r="A0" s="0" t="inlineStr">
+        <is>
+          <t>양념치킨</t>
+        </is>
+      </c>
+      <c r="B0" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C0" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D0" s="0" t="n">
+        <v>18000</v>
+      </c>
+      <c r="E0" s="0" t="inlineStr"/>
+    </row>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>닭볶음탕</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>양념치킨</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>삼겹살</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>김밥</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>된장국</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D3" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="0" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -548,36 +543,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>삼겹살</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -588,36 +561,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>오징어튀김</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>2600</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" t="n">
-        <v>2600</v>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
edit c_click --None issue
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -359,36 +359,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>양념치킨</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -399,36 +377,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>양념치킨</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E1" s="0" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
edit c_click None issue
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E2"/>
+  <dimension ref="A2:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,6 +406,48 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>치킨</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>대패삼겹살</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -453,14 +495,36 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>맥주</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add personal info -room info
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,140 +385,120 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
+    <row r="1"/>
     <row r="2">
-      <c r="A2" s="0" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>치즈김밥</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>대패삼겹살</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>맥주</t>
         </is>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B1" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>치킨</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="C1" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>대패삼겹살</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E4" s="0" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>맥주</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
+      <c r="D1" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>

</xml_diff>

<commit_message>
edit set() --has a bunch of trubles
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -349,7 +349,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="18.5" customWidth="1" style="3" min="4" max="4"/>
   </cols>
@@ -581,96 +581,6 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -680,94 +590,144 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>삼겹살</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" t="n">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>치즈김밥</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>식탁보</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>6000</v>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>식탁보</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="n">
-        <v>18000</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>치즈김밥</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>김밥</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
add final in main
</commit_message>
<xml_diff>
--- a/xl/personal.xlsx
+++ b/xl/personal.xlsx
@@ -349,7 +349,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="18.5" customWidth="1" style="3" min="4" max="4"/>
   </cols>
@@ -360,34 +360,90 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr"/>
-      <c r="C1" s="1" t="inlineStr"/>
-      <c r="D1" s="1" t="inlineStr"/>
-      <c r="E1" s="0" t="inlineStr"/>
-      <c r="F1" s="0" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr"/>
-      <c r="C2" s="1" t="inlineStr"/>
-      <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="0" t="inlineStr"/>
-      <c r="F2" s="0" t="inlineStr"/>
+          <t>233</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr"/>
-      <c r="C3" s="1" t="inlineStr"/>
-      <c r="D3" s="2" t="inlineStr"/>
-      <c r="E3" s="0" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
       <c r="F3" s="0" t="inlineStr"/>
     </row>
     <row r="4">

</xml_diff>